<commit_message>
Added some modeling tools and ecel document to import json data to.
</commit_message>
<xml_diff>
--- a/SimResultsGraphs.xlsx
+++ b/SimResultsGraphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Documents\programming\projects\visual-studio\LineServiceSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{648CED6F-98A6-436E-AD3D-F0F966C37E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C30E51D-B219-4A84-BD13-BA0F8CF04599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DA9FA37F-384F-4A39-9F67-7404FC5CD0D2}"/>
   </bookViews>
@@ -6912,8 +6912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9976B758-C8F2-445C-812D-617907C64460}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>